<commit_message>
Con estos cambios, el archivo ya no ordenará los datos ni por la columna Debe ni por Haber, ni por Indice_Punteo.
</commit_message>
<xml_diff>
--- a/informes/Puntear/Puntear_punteados.xlsx
+++ b/informes/Puntear/Puntear_punteados.xlsx
@@ -595,14 +595,14 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45589</v>
+        <v>45588</v>
       </c>
       <c r="B3" t="n">
-        <v>4039117</v>
+        <v>4038810</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409099909/1</t>
+          <t>Creación Anticipo 409103089/1</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -614,20 +614,20 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2665.29</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2615.42</v>
       </c>
       <c r="H3" t="n">
-        <v>-2615.42</v>
+        <v>-5280.71</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Ana P</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -655,23 +655,23 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>409099909/1</t>
+          <t>409103089/1</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45638</v>
+        <v>45589</v>
       </c>
       <c r="B4" t="n">
-        <v>4046012</v>
+        <v>4039117</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409120147/1</t>
+          <t>Compensación Anticipo 409099909/1</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -683,13 +683,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>370.19</v>
+        <v>2665.29</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>-465.55</v>
+        <v>-2615.42</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -724,23 +724,23 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>409120147/1</t>
+          <t>409099909/1</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45631</v>
+        <v>45600</v>
       </c>
       <c r="B5" t="n">
-        <v>4045143</v>
+        <v>4040429</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409120147/1</t>
+          <t>Compensación Anticipo 409103089/1</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -752,20 +752,20 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>2448.73</v>
       </c>
       <c r="G5" t="n">
-        <v>370.19</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>-835.74</v>
+        <v>-166.69</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -793,11 +793,11 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>409120147/1</t>
+          <t>409103089/1</t>
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -871,14 +871,14 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45600</v>
+        <v>45602</v>
       </c>
       <c r="B7" t="n">
-        <v>4040429</v>
+        <v>4040707</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409103089/1</t>
+          <t>Creación Anticipo 409108164/1</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -890,20 +890,20 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2448.73</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>2653.64</v>
       </c>
       <c r="H7" t="n">
-        <v>-166.69</v>
+        <v>-2653.64</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -931,23 +931,23 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>409103089/1</t>
+          <t>409108164/1</t>
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45588</v>
+        <v>45602</v>
       </c>
       <c r="B8" t="n">
-        <v>4038810</v>
+        <v>4040708</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409103089/1</t>
+          <t>Creación Anticipo 409108165/1</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -962,10 +962,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>2615.42</v>
+        <v>313.56</v>
       </c>
       <c r="H8" t="n">
-        <v>-5280.71</v>
+        <v>-2967.2</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1000,23 +1000,23 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>409103089/1</t>
+          <t>409108165/1</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45602</v>
+        <v>45603</v>
       </c>
       <c r="B9" t="n">
-        <v>4040707</v>
+        <v>4040969</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409108164/1</t>
+          <t>Compensación Anticipo 409108165/1</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -1028,20 +1028,20 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>164.08</v>
       </c>
       <c r="G9" t="n">
-        <v>2653.64</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>-2653.64</v>
+        <v>-2803.12</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1069,11 +1069,11 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>409108164/1</t>
+          <t>409108165/1</t>
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -1147,14 +1147,14 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45611</v>
+        <v>45610</v>
       </c>
       <c r="B11" t="n">
-        <v>4042137</v>
+        <v>4041906</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409108164/1</t>
+          <t>Compensación Anticipo 409108165/1</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -1166,20 +1166,20 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1642.72</v>
+        <v>149.48</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>-827.49</v>
+        <v>-2108.27</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>Ana P</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1207,23 +1207,23 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>409108164/1</t>
+          <t>409108165/1</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45642</v>
+        <v>45611</v>
       </c>
       <c r="B12" t="n">
-        <v>4046527</v>
+        <v>4042080</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409108164/1</t>
+          <t>Creación Anticipo 409112186/1</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1235,20 +1235,20 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>465.55</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>361.94</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>-2470.21</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1276,23 +1276,23 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>409108164/1</t>
+          <t>409112186/1</t>
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45603</v>
+        <v>45611</v>
       </c>
       <c r="B13" t="n">
-        <v>4040969</v>
+        <v>4042137</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409108165/1</t>
+          <t>Compensación Anticipo 409108164/1</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1304,20 +1304,20 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>164.08</v>
+        <v>1642.72</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>-2803.12</v>
+        <v>-827.49</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1345,23 +1345,23 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>409108165/1</t>
+          <t>409108164/1</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45610</v>
+        <v>45616</v>
       </c>
       <c r="B14" t="n">
-        <v>4041906</v>
+        <v>4042912</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409108165/1</t>
+          <t>Compensación Anticipo 409112186/1</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1373,20 +1373,20 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>149.48</v>
+        <v>105.9</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>-2108.27</v>
+        <v>-721.59</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Ana P</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1414,23 +1414,23 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>409108165/1</t>
+          <t>409112186/1</t>
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45602</v>
+        <v>45621</v>
       </c>
       <c r="B15" t="n">
-        <v>4040708</v>
+        <v>4043419</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409108165/1</t>
+          <t>Compensación Anticipo 409112186/1</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1442,20 +1442,20 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>256.04</v>
       </c>
       <c r="G15" t="n">
-        <v>313.56</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>-2967.2</v>
+        <v>-465.55</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1483,23 +1483,23 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>409108165/1</t>
+          <t>409112186/1</t>
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45621</v>
+        <v>45631</v>
       </c>
       <c r="B16" t="n">
-        <v>4043419</v>
+        <v>4045143</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409112186/1</t>
+          <t>Creación Anticipo 409120147/1</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1511,20 +1511,20 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>256.04</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>370.19</v>
       </c>
       <c r="H16" t="n">
-        <v>-465.55</v>
+        <v>-835.74</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1552,23 +1552,23 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>409112186/1</t>
+          <t>409120147/1</t>
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45611</v>
+        <v>45638</v>
       </c>
       <c r="B17" t="n">
-        <v>4042080</v>
+        <v>4046012</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409112186/1</t>
+          <t>Compensación Anticipo 409120147/1</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1580,20 +1580,20 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>370.19</v>
       </c>
       <c r="G17" t="n">
-        <v>361.94</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>-2470.21</v>
+        <v>-465.55</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>Ana P</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1621,23 +1621,23 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>409112186/1</t>
+          <t>409120147/1</t>
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45616</v>
+        <v>45642</v>
       </c>
       <c r="B18" t="n">
-        <v>4042912</v>
+        <v>4046527</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409112186/1</t>
+          <t>Compensación Anticipo 409108164/1</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1649,13 +1649,13 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>105.9</v>
+        <v>465.55</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>-721.59</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1690,11 +1690,11 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>409112186/1</t>
+          <t>409108164/1</t>
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>